<commit_message>
Switch parallel processing and parse results
</commit_message>
<xml_diff>
--- a/test/bbox.xlsx
+++ b/test/bbox.xlsx
@@ -466,236 +466,236 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>211</v>
+      </c>
+      <c r="B2" t="n">
+        <v>236</v>
+      </c>
+      <c r="C2" t="n">
         <v>191</v>
       </c>
-      <c r="B2" t="n">
+      <c r="D2" t="n">
         <v>232</v>
       </c>
-      <c r="C2" t="n">
+      <c r="E2" t="n">
         <v>195</v>
       </c>
-      <c r="D2" t="n">
+      <c r="F2" t="n">
         <v>204</v>
       </c>
-      <c r="E2" t="n">
+      <c r="G2" t="n">
         <v>216</v>
       </c>
-      <c r="F2" t="n">
+      <c r="H2" t="n">
         <v>207</v>
-      </c>
-      <c r="G2" t="n">
-        <v>211</v>
-      </c>
-      <c r="H2" t="n">
-        <v>236</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
+        <v>239</v>
+      </c>
+      <c r="B3" t="n">
+        <v>218</v>
+      </c>
+      <c r="C3" t="n">
         <v>211</v>
       </c>
-      <c r="B3" t="n">
+      <c r="D3" t="n">
+        <v>218</v>
+      </c>
+      <c r="E3" t="n">
+        <v>211</v>
+      </c>
+      <c r="F3" t="n">
         <v>195</v>
       </c>
-      <c r="C3" t="n">
+      <c r="G3" t="n">
         <v>239</v>
       </c>
-      <c r="D3" t="n">
+      <c r="H3" t="n">
         <v>195</v>
-      </c>
-      <c r="E3" t="n">
-        <v>239</v>
-      </c>
-      <c r="F3" t="n">
-        <v>218</v>
-      </c>
-      <c r="G3" t="n">
-        <v>211</v>
-      </c>
-      <c r="H3" t="n">
-        <v>218</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
+        <v>184</v>
+      </c>
+      <c r="B4" t="n">
+        <v>278</v>
+      </c>
+      <c r="C4" t="n">
         <v>158</v>
       </c>
-      <c r="B4" t="n">
+      <c r="D4" t="n">
+        <v>278</v>
+      </c>
+      <c r="E4" t="n">
+        <v>158</v>
+      </c>
+      <c r="F4" t="n">
         <v>241</v>
       </c>
-      <c r="C4" t="n">
+      <c r="G4" t="n">
         <v>184</v>
       </c>
-      <c r="D4" t="n">
+      <c r="H4" t="n">
         <v>241</v>
-      </c>
-      <c r="E4" t="n">
-        <v>184</v>
-      </c>
-      <c r="F4" t="n">
-        <v>278</v>
-      </c>
-      <c r="G4" t="n">
-        <v>158</v>
-      </c>
-      <c r="H4" t="n">
-        <v>278</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
+        <v>165</v>
+      </c>
+      <c r="B5" t="n">
+        <v>247</v>
+      </c>
+      <c r="C5" t="n">
         <v>155</v>
       </c>
-      <c r="B5" t="n">
+      <c r="D5" t="n">
         <v>202</v>
       </c>
-      <c r="C5" t="n">
+      <c r="E5" t="n">
         <v>189</v>
       </c>
-      <c r="D5" t="n">
+      <c r="F5" t="n">
         <v>194</v>
       </c>
-      <c r="E5" t="n">
+      <c r="G5" t="n">
         <v>199</v>
       </c>
-      <c r="F5" t="n">
+      <c r="H5" t="n">
         <v>240</v>
-      </c>
-      <c r="G5" t="n">
-        <v>165</v>
-      </c>
-      <c r="H5" t="n">
-        <v>247</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
+        <v>213</v>
+      </c>
+      <c r="B6" t="n">
+        <v>297</v>
+      </c>
+      <c r="C6" t="n">
         <v>174</v>
       </c>
-      <c r="B6" t="n">
+      <c r="D6" t="n">
         <v>271</v>
       </c>
-      <c r="C6" t="n">
+      <c r="E6" t="n">
         <v>196</v>
       </c>
-      <c r="D6" t="n">
+      <c r="F6" t="n">
         <v>238</v>
       </c>
-      <c r="E6" t="n">
+      <c r="G6" t="n">
         <v>235</v>
       </c>
-      <c r="F6" t="n">
+      <c r="H6" t="n">
         <v>264</v>
-      </c>
-      <c r="G6" t="n">
-        <v>213</v>
-      </c>
-      <c r="H6" t="n">
-        <v>297</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
+        <v>199</v>
+      </c>
+      <c r="B7" t="n">
+        <v>206</v>
+      </c>
+      <c r="C7" t="n">
         <v>181</v>
       </c>
-      <c r="B7" t="n">
+      <c r="D7" t="n">
         <v>158</v>
       </c>
-      <c r="C7" t="n">
+      <c r="E7" t="n">
         <v>227</v>
       </c>
-      <c r="D7" t="n">
+      <c r="F7" t="n">
         <v>141</v>
       </c>
-      <c r="E7" t="n">
+      <c r="G7" t="n">
         <v>245</v>
       </c>
-      <c r="F7" t="n">
+      <c r="H7" t="n">
         <v>189</v>
-      </c>
-      <c r="G7" t="n">
-        <v>199</v>
-      </c>
-      <c r="H7" t="n">
-        <v>206</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
+        <v>227</v>
+      </c>
+      <c r="B8" t="n">
+        <v>281</v>
+      </c>
+      <c r="C8" t="n">
         <v>211</v>
       </c>
-      <c r="B8" t="n">
+      <c r="D8" t="n">
         <v>233</v>
       </c>
-      <c r="C8" t="n">
+      <c r="E8" t="n">
         <v>277</v>
       </c>
-      <c r="D8" t="n">
+      <c r="F8" t="n">
         <v>210</v>
       </c>
-      <c r="E8" t="n">
+      <c r="G8" t="n">
         <v>294</v>
       </c>
-      <c r="F8" t="n">
+      <c r="H8" t="n">
         <v>258</v>
-      </c>
-      <c r="G8" t="n">
-        <v>227</v>
-      </c>
-      <c r="H8" t="n">
-        <v>281</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
+        <v>164</v>
+      </c>
+      <c r="B9" t="n">
+        <v>203</v>
+      </c>
+      <c r="C9" t="n">
         <v>94</v>
       </c>
-      <c r="B9" t="n">
+      <c r="D9" t="n">
         <v>199</v>
       </c>
-      <c r="C9" t="n">
+      <c r="E9" t="n">
         <v>96</v>
       </c>
-      <c r="D9" t="n">
+      <c r="F9" t="n">
         <v>148</v>
       </c>
-      <c r="E9" t="n">
+      <c r="G9" t="n">
         <v>167</v>
       </c>
-      <c r="F9" t="n">
+      <c r="H9" t="n">
         <v>151</v>
-      </c>
-      <c r="G9" t="n">
-        <v>164</v>
-      </c>
-      <c r="H9" t="n">
-        <v>203</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
+        <v>103</v>
+      </c>
+      <c r="B10" t="n">
+        <v>293</v>
+      </c>
+      <c r="C10" t="n">
         <v>99</v>
       </c>
-      <c r="B10" t="n">
+      <c r="D10" t="n">
         <v>241</v>
       </c>
-      <c r="C10" t="n">
+      <c r="E10" t="n">
         <v>166</v>
       </c>
-      <c r="D10" t="n">
+      <c r="F10" t="n">
         <v>235</v>
       </c>
-      <c r="E10" t="n">
+      <c r="G10" t="n">
         <v>170</v>
       </c>
-      <c r="F10" t="n">
+      <c r="H10" t="n">
         <v>288</v>
-      </c>
-      <c r="G10" t="n">
-        <v>103</v>
-      </c>
-      <c r="H10" t="n">
-        <v>293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>